<commit_message>
Update purchase link of bearing.
</commit_message>
<xml_diff>
--- a/1.RobotModel/Parts-Purchased/BOM.xlsx
+++ b/1.RobotModel/Parts-Purchased/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22193" windowHeight="10470"/>
+    <workbookView windowWidth="30720" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
     <t>https://detail.tmall.com/item.htm?id=611796709407&amp;spm=a1z09.2.0.0.6f8c2e8daIyqdB&amp;_u=k2st8hc2e6c7</t>
   </si>
   <si>
-    <t>2*6*3</t>
+    <t>3*6*2</t>
   </si>
   <si>
     <t>s</t>
@@ -804,7 +804,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -815,12 +815,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1351,16 +1345,16 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.1" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.84259259259259" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="16.2105263157895" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.212962962963" style="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6315789473684" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.5263157894737" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8421052631579" style="1"/>
+    <col min="3" max="3" width="24.6296296296296" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5277777777778" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.84259259259259" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1423,7 +1417,7 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1437,7 +1431,7 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1496,7 +1490,7 @@
       <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="1">

</xml_diff>